<commit_message>
Changed rule for claiming health and wellness bills
</commit_message>
<xml_diff>
--- a/src/main/resources/payrollFiles/HealthAndBroadband.xlsx
+++ b/src/main/resources/payrollFiles/HealthAndBroadband.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -31,7 +31,10 @@
     <t xml:space="preserve">Broadband</t>
   </si>
   <si>
-    <t xml:space="preserve">Activation Date</t>
+    <t xml:space="preserve">Activation Date For Health ( Joining Date )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activation Date For Broadband ( Financial Year )</t>
   </si>
   <si>
     <t xml:space="preserve">Last Claimed Date For Health</t>
@@ -40,10 +43,25 @@
     <t xml:space="preserve">Last Claimed Date For Broadband</t>
   </si>
   <si>
+    <t xml:space="preserve">duplicate@testvagrant.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JoiningDate (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinancialYearDate (dd/mm/yyyy)</t>
+  </si>
+  <si>
     <t xml:space="preserve">radhakrishnan@testvagrant.com</t>
   </si>
   <si>
-    <t xml:space="preserve">4000</t>
+    <t xml:space="preserve">10/02/2018</t>
   </si>
   <si>
     <t xml:space="preserve">01/04/2018</t>
@@ -52,16 +70,16 @@
     <t xml:space="preserve">abhishek@testvagrant.com</t>
   </si>
   <si>
-    <t xml:space="preserve">01/10/2018</t>
+    <t xml:space="preserve">01/01/2018</t>
   </si>
   <si>
     <t xml:space="preserve">vaibhav@testvagrant.com</t>
   </si>
   <si>
-    <t xml:space="preserve">6000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12000</t>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/06/2018</t>
   </si>
 </sst>
 </file>
@@ -73,7 +91,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -102,12 +120,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -161,15 +173,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,22 +206,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="29.5" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="24.87" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="21.5" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="17.13" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="25.1" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="27.42" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="32.57" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="1025" customWidth="true" hidden="false" style="0" width="8.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -221,78 +238,113 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>12000</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>43121.5844582986</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>42519.6564467593</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>42370.0423726852</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>42370.0423726852</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>43121.5844582986</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>42519.6564467593</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>9000</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>42519.6564467593</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>43117.9666390625</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>7000</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>42519.6564467593</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>43117.9666390625</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>11049.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>43238.65097244213</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>43238.650704768515</v>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>43238.6509724421</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>43238.6507047685</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="radhakrishnan@testvagrant.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="abhishek@testvagrant.com"/>
-    <hyperlink ref="A4" r:id="rId3" display="vaibhav@testvagrant.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="duplicate@testvagrant.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="radhakrishnan@testvagrant.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="abhishek@testvagrant.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>